<commit_message>
Added row for n=100
</commit_message>
<xml_diff>
--- a/resources/test-results.xlsx
+++ b/resources/test-results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Evan\Projects\intellij-projects\powerset-test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{96ADCACC-F236-4473-ADD5-F45DE2B44DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9904852B-C182-40F9-ACA1-4E1927779A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8810" yWindow="3800" windowWidth="28800" windowHeight="15370" xr2:uid="{BC6CF1DA-04B1-49BE-B095-01B6E9F33F1E}"/>
+    <workbookView xWindow="4390" yWindow="1270" windowWidth="28800" windowHeight="15370" xr2:uid="{BC6CF1DA-04B1-49BE-B095-01B6E9F33F1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Powerset Calculations" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>n</t>
   </si>
@@ -95,6 +95,9 @@
 than Integer.MAX_VALUE number of objects. ConcurrentHashMap provides a mappingCount()
 method which is more accurate than size().
 This was tested on a server with ~500G of RAM. The JVM running had access to 497G of RAM inside a docker container. Any negative "Used" memory values are a delta caused by a manual call to the garbage collector.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;-- Greater than Long.MAX_VALUE</t>
   </si>
 </sst>
 </file>
@@ -329,9 +332,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -341,6 +341,27 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -350,32 +371,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -388,7 +389,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -402,6 +403,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -730,229 +737,228 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9E5C38A-79B2-4DE1-9D2F-F3BC66073D3E}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="1"/>
-    <col min="2" max="3" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="7" t="s">
+      <c r="C1" s="17"/>
+      <c r="D1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="9"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:8" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>5</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <f>2^A3</f>
         <v>32</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>32</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>508847</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>508879</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="27">
         <f t="shared" ref="F3:F6" si="0">(D3-E3)/1024</f>
         <v>-3.125E-2</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>10</v>
       </c>
-      <c r="B4" s="5">
-        <f t="shared" ref="B4:B10" si="1">2^A4</f>
+      <c r="B4" s="4">
+        <f t="shared" ref="B4:B11" si="1">2^A4</f>
         <v>1024</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>1024</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>508832</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>508879</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="27">
         <f t="shared" si="0"/>
         <v>-4.58984375E-2</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>15</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <f t="shared" si="1"/>
         <v>32768</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>32768</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>508847</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>508895</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="27">
         <f t="shared" si="0"/>
         <v>-4.6875E-2</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>20</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <f t="shared" si="1"/>
         <v>1048576</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>1048576</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>508847</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>508607</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="27">
         <f t="shared" si="0"/>
         <v>0.234375</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>25</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <f t="shared" si="1"/>
         <v>33554432</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>33554432</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>508847</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>498815</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="27">
         <f>(D7-E7)/1024</f>
         <v>9.796875</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>30</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <f t="shared" si="1"/>
         <v>1073741824</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>1073741824</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>508847</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>264767</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="27">
         <f t="shared" ref="F8:F9" si="2">(D8-E8)/1024</f>
         <v>238.359375</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A9" s="16">
+      <c r="A9" s="10">
         <v>31</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="11">
         <f t="shared" si="1"/>
         <v>2147483648</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="11">
         <v>2147483648</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="11">
         <v>508863</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="11">
         <v>48689</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="28">
         <f t="shared" si="2"/>
         <v>449.388671875</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="12" t="s">
         <v>10</v>
       </c>
       <c r="H9" s="1" t="s">
@@ -960,133 +966,160 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A10" s="6">
+      <c r="A10" s="5">
         <v>32</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <f t="shared" si="1"/>
         <v>4294967296</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>508847</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="A11" s="5">
+        <v>100</v>
+      </c>
+      <c r="B11" s="5">
+        <f t="shared" si="1"/>
+        <v>1.2676506002282294E+30</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5">
+        <v>508847</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="20" t="s">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="22"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A14" s="23"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="25"/>
-    </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="23"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="25"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A16" s="23"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="25"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="20"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A15" s="21"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="23"/>
+    </row>
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="21"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="23"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A17" s="23"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="25"/>
+      <c r="A17" s="21"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="23"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A18" s="23"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="25"/>
-    </row>
-    <row r="19" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="23"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="25"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A20" s="23"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="25"/>
+      <c r="A18" s="21"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="23"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A19" s="21"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="23"/>
+    </row>
+    <row r="20" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="21"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="23"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A21" s="26"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="28"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="23"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A22" s="24"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="A13:G21"/>
+    <mergeCell ref="A14:G22"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:E10 G7:G10">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">

</xml_diff>

<commit_message>
Updated README and charts
</commit_message>
<xml_diff>
--- a/resources/test-results.xlsx
+++ b/resources/test-results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Evan\Projects\intellij-projects\powerset-test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242C1336-68C1-49A8-B962-845EEBCCC372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6020A6A8-D0F6-4AD7-9FBA-EC9525E3589A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8400" yWindow="3110" windowWidth="28800" windowHeight="15370" xr2:uid="{BC6CF1DA-04B1-49BE-B095-01B6E9F33F1E}"/>
+    <workbookView xWindow="8400" yWindow="3110" windowWidth="28800" windowHeight="15370" activeTab="1" xr2:uid="{BC6CF1DA-04B1-49BE-B095-01B6E9F33F1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Powerset with BitSet" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="25">
   <si>
     <t>n</t>
   </si>
@@ -344,7 +344,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -426,6 +426,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -763,11 +767,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9E5C38A-79B2-4DE1-9D2F-F3BC66073D3E}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
   <cols>
@@ -792,7 +794,7 @@
       <c r="E1" s="16"/>
       <c r="F1" s="17"/>
     </row>
-    <row r="2" spans="1:8" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -815,7 +817,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" ht="15.5" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A3" s="4">
         <v>5</v>
       </c>
@@ -840,12 +842,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" s="4">
         <v>10</v>
       </c>
       <c r="B4" s="4">
-        <f t="shared" ref="B4:B12" si="1">2^A4</f>
+        <f t="shared" ref="B4:B13" si="1">2^A4</f>
         <v>1024</v>
       </c>
       <c r="C4" s="4">
@@ -865,7 +867,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" s="4">
         <v>15</v>
       </c>
@@ -890,7 +892,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" s="4">
         <v>20</v>
       </c>
@@ -1019,17 +1021,17 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11" s="5">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="B11" s="5">
         <f t="shared" si="1"/>
-        <v>9.2233720368547758E+18</v>
+        <v>8589934592</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="5">
-        <v>508847</v>
+      <c r="D11" s="29">
+        <v>508863</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>1</v>
@@ -1039,18 +1041,15 @@
       </c>
       <c r="G11" s="5" t="s">
         <v>1</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A12" s="5">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="B12" s="5">
         <f t="shared" si="1"/>
-        <v>1.2676506002282294E+30</v>
+        <v>9.2233720368547758E+18</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>1</v>
@@ -1067,14 +1066,33 @@
       <c r="G12" s="5" t="s">
         <v>1</v>
       </c>
+      <c r="H12" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="A13" s="5">
+        <v>100</v>
+      </c>
+      <c r="B13" s="5">
+        <f t="shared" si="1"/>
+        <v>1.2676506002282294E+30</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="5">
+        <v>508847</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14" s="2"/>
@@ -1084,27 +1102,26 @@
       <c r="E14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="20" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A16" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="22"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A16" s="23"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="25"/>
-    </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="22"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="23"/>
       <c r="B17" s="24"/>
       <c r="C17" s="24"/>
@@ -1140,7 +1157,7 @@
       <c r="F20" s="24"/>
       <c r="G20" s="25"/>
     </row>
-    <row r="21" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" s="23"/>
       <c r="B21" s="24"/>
       <c r="C21" s="24"/>
@@ -1159,21 +1176,30 @@
       <c r="G22" s="25"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A23" s="26"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="28"/>
+      <c r="A23" s="23"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="25"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A24" s="26"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="A15:G23"/>
+    <mergeCell ref="A16:G24"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:E11 G7:G11">
+  <conditionalFormatting sqref="G7:G12 D7:E12">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"CRASH"</formula>
     </cfRule>
@@ -1185,10 +1211,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{597AFF86-F51A-4023-AFD3-AD70CE89348E}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1202,7 +1228,7 @@
     <col min="7" max="7" width="15.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
       <c r="B1" s="18" t="s">
         <v>7</v>
@@ -1215,7 +1241,7 @@
       <c r="F1" s="17"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1238,7 +1264,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.5" thickTop="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" ht="15.5" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A3" s="4">
         <v>5</v>
       </c>
@@ -1263,12 +1289,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.4">
       <c r="A4" s="4">
         <v>10</v>
       </c>
       <c r="B4" s="4">
-        <f t="shared" ref="B4:B12" si="1">2^A4</f>
+        <f t="shared" ref="B4:B13" si="1">2^A4</f>
         <v>1024</v>
       </c>
       <c r="C4" s="4">
@@ -1288,7 +1314,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.4">
       <c r="A5" s="4">
         <v>15</v>
       </c>
@@ -1313,7 +1339,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.4">
       <c r="A6" s="4">
         <v>20</v>
       </c>
@@ -1338,7 +1364,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.4">
       <c r="A7" s="4">
         <v>25</v>
       </c>
@@ -1363,7 +1389,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.4">
       <c r="A8" s="4">
         <v>30</v>
       </c>
@@ -1388,7 +1414,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.4">
       <c r="A9" s="10">
         <v>31</v>
       </c>
@@ -1416,7 +1442,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.4">
       <c r="A10" s="4">
         <v>32</v>
       </c>
@@ -1441,7 +1467,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.4">
       <c r="A11" s="5">
         <v>33</v>
       </c>
@@ -1452,8 +1478,8 @@
       <c r="C11" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>1</v>
+      <c r="D11" s="5">
+        <v>508847</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>1</v>
@@ -1465,40 +1491,61 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.4">
       <c r="A12" s="5">
+        <v>63</v>
+      </c>
+      <c r="B12" s="5">
+        <f t="shared" si="1"/>
+        <v>9.2233720368547758E+18</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="5">
+        <v>508847</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+    </row>
+    <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.4">
+      <c r="A13" s="5">
         <v>100</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B13" s="5">
         <f t="shared" si="1"/>
         <v>1.2676506002282294E+30</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.4">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.4">
+      <c r="C13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="5">
+        <v>508847</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.4">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1507,25 +1554,25 @@
       <c r="F14" s="3"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="20" t="s">
+    <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.4">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="22"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="23"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="25"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="22"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="23"/>
@@ -1582,21 +1629,31 @@
       <c r="G22" s="25"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="26"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="28"/>
+      <c r="A23" s="23"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="25"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="26"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A15:G23"/>
+    <mergeCell ref="A16:G24"/>
+    <mergeCell ref="H12:K12"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:E11 G7:G11">
+  <conditionalFormatting sqref="D7:E12 G7:G12 H12">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"CRASH"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Reduced memory footprint by reducing object alignment in memory
</commit_message>
<xml_diff>
--- a/resources/test-results.xlsx
+++ b/resources/test-results.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Evan\Projects\intellij-projects\powerset-test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6020A6A8-D0F6-4AD7-9FBA-EC9525E3589A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F69E86-B065-417A-967D-1D310693427F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8400" yWindow="3110" windowWidth="28800" windowHeight="15370" activeTab="1" xr2:uid="{BC6CF1DA-04B1-49BE-B095-01B6E9F33F1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Powerset with BitSet" sheetId="1" r:id="rId1"/>
-    <sheet name="Powerset with Counter" sheetId="2" r:id="rId2"/>
+    <sheet name="Powerset with Counter" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="21">
   <si>
     <t>n</t>
   </si>
@@ -46,12 +46,6 @@
     <t>Elapsed Time</t>
   </si>
   <si>
-    <t>0m 15s</t>
-  </si>
-  <si>
-    <t>4m 52s</t>
-  </si>
-  <si>
     <t>Memory</t>
   </si>
   <si>
@@ -65,21 +59,6 @@
   </si>
   <si>
     <t>Enumerated</t>
-  </si>
-  <si>
-    <t>7m  7s</t>
-  </si>
-  <si>
-    <t>0m  4s</t>
-  </si>
-  <si>
-    <t>0m  3s</t>
-  </si>
-  <si>
-    <t>0m  5s</t>
-  </si>
-  <si>
-    <t>0m  1s</t>
   </si>
   <si>
     <t xml:space="preserve"> &lt;-- Integer.MAX_VALUE + 1</t>
@@ -104,16 +83,25 @@
     <t>0m  2s</t>
   </si>
   <si>
-    <t>1m 27s</t>
-  </si>
-  <si>
-    <t>2m 30s</t>
-  </si>
-  <si>
-    <t>6m 58s</t>
-  </si>
-  <si>
     <t xml:space="preserve"> &lt;-- Long.MAX_VALUE + 1</t>
+  </si>
+  <si>
+    <t>5m 07s</t>
+  </si>
+  <si>
+    <t>2m 23s</t>
+  </si>
+  <si>
+    <t>1m 05s</t>
+  </si>
+  <si>
+    <t>0m  6s</t>
+  </si>
+  <si>
+    <t>4m  4s</t>
+  </si>
+  <si>
+    <t>5m 49s</t>
   </si>
 </sst>
 </file>
@@ -384,6 +372,9 @@
     <xf numFmtId="2" fontId="4" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -426,10 +417,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -769,7 +757,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9E5C38A-79B2-4DE1-9D2F-F3BC66073D3E}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
   <cols>
@@ -784,34 +774,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B1" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="15" t="s">
+      <c r="B1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="F1" s="17"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="17"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:8" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>16</v>
-      </c>
       <c r="E2" s="6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>2</v>
@@ -829,17 +819,17 @@
         <v>32</v>
       </c>
       <c r="D3" s="4">
-        <v>508847</v>
+        <v>508910</v>
       </c>
       <c r="E3" s="4">
-        <v>508879</v>
+        <v>508926</v>
       </c>
       <c r="F3" s="13">
         <f t="shared" ref="F3:F6" si="0">(D3-E3)/1024</f>
-        <v>-3.125E-2</v>
+        <v>-1.5625E-2</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.4">
@@ -854,14 +844,14 @@
         <v>1024</v>
       </c>
       <c r="D4" s="4">
-        <v>508832</v>
+        <v>508926</v>
       </c>
       <c r="E4" s="4">
-        <v>508879</v>
+        <v>508926</v>
       </c>
       <c r="F4" s="13">
         <f t="shared" si="0"/>
-        <v>-4.58984375E-2</v>
+        <v>0</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>12</v>
@@ -879,17 +869,17 @@
         <v>32768</v>
       </c>
       <c r="D5" s="4">
-        <v>508847</v>
+        <v>508926</v>
       </c>
       <c r="E5" s="4">
-        <v>508895</v>
+        <v>508922</v>
       </c>
       <c r="F5" s="13">
         <f t="shared" si="0"/>
-        <v>-4.6875E-2</v>
+        <v>3.90625E-3</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.4">
@@ -904,17 +894,17 @@
         <v>1048576</v>
       </c>
       <c r="D6" s="4">
-        <v>508847</v>
+        <v>508926</v>
       </c>
       <c r="E6" s="4">
-        <v>508607</v>
+        <v>508798</v>
       </c>
       <c r="F6" s="13">
         <f t="shared" si="0"/>
-        <v>0.234375</v>
+        <v>0.125</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.4">
@@ -929,17 +919,17 @@
         <v>33554432</v>
       </c>
       <c r="D7" s="4">
-        <v>508847</v>
+        <v>508926</v>
       </c>
       <c r="E7" s="4">
-        <v>498815</v>
+        <v>505310</v>
       </c>
       <c r="F7" s="13">
         <f>(D7-E7)/1024</f>
-        <v>9.796875</v>
+        <v>3.53125</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.4">
@@ -954,17 +944,17 @@
         <v>1073741824</v>
       </c>
       <c r="D8" s="4">
-        <v>508847</v>
+        <v>508926</v>
       </c>
       <c r="E8" s="4">
-        <v>264767</v>
+        <v>402168</v>
       </c>
       <c r="F8" s="13">
         <f t="shared" ref="F8:F9" si="2">(D8-E8)/1024</f>
-        <v>238.359375</v>
+        <v>104.255859375</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.4">
@@ -979,20 +969,20 @@
         <v>2147483648</v>
       </c>
       <c r="D9" s="11">
-        <v>508863</v>
+        <v>508926</v>
       </c>
       <c r="E9" s="11">
-        <v>48689</v>
+        <v>304042</v>
       </c>
       <c r="F9" s="14">
         <f t="shared" si="2"/>
-        <v>449.388671875</v>
+        <v>200.08203125</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.4">
@@ -1006,12 +996,8 @@
       <c r="C10" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="5">
-        <v>508847</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
       <c r="F10" s="9" t="s">
         <v>1</v>
       </c>
@@ -1030,12 +1016,8 @@
       <c r="C11" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="29">
-        <v>508863</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="D11" s="15"/>
+      <c r="E11" s="5"/>
       <c r="F11" s="9" t="s">
         <v>1</v>
       </c>
@@ -1054,12 +1036,8 @@
       <c r="C12" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="5">
-        <v>508847</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
       <c r="F12" s="9" t="s">
         <v>1</v>
       </c>
@@ -1067,7 +1045,7 @@
         <v>1</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.4">
@@ -1081,12 +1059,8 @@
       <c r="C13" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="5">
-        <v>508847</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
       <c r="F13" s="9" t="s">
         <v>1</v>
       </c>
@@ -1111,87 +1085,87 @@
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A16" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="22"/>
+      <c r="A16" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="23"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A17" s="23"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="25"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="26"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A18" s="23"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="25"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="26"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A19" s="23"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="25"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="26"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A20" s="23"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="25"/>
+      <c r="A20" s="24"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="26"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A21" s="23"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="25"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="26"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A22" s="23"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="25"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="26"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A23" s="23"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="25"/>
+      <c r="A23" s="24"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="26"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A24" s="26"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="28"/>
+      <c r="A24" s="27"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1199,7 +1173,7 @@
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="A16:G24"/>
   </mergeCells>
-  <conditionalFormatting sqref="G7:G12 D7:E12">
+  <conditionalFormatting sqref="D7:E12 G7:G12">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"CRASH"</formula>
     </cfRule>
@@ -1210,55 +1184,55 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{597AFF86-F51A-4023-AFD3-AD70CE89348E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FA34550-6DDB-4D44-BC4D-A7B746848E22}">
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" customWidth="1"/>
-    <col min="2" max="2" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.4">
-      <c r="A1" s="1"/>
-      <c r="B1" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="15" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="B1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="1"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="17"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>16</v>
-      </c>
       <c r="E2" s="6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>2</v>
@@ -1276,214 +1250,208 @@
         <v>32</v>
       </c>
       <c r="D3" s="4">
-        <v>508863</v>
+        <v>508910</v>
       </c>
       <c r="E3" s="4">
-        <v>508863</v>
+        <v>508926</v>
       </c>
       <c r="F3" s="13">
-        <f t="shared" ref="F3:F10" si="0">(D3-E3)/1024</f>
-        <v>0</v>
+        <f>(D3-E3)/1024</f>
+        <v>-1.5625E-2</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="4">
         <v>10</v>
       </c>
       <c r="B4" s="4">
-        <f t="shared" ref="B4:B13" si="1">2^A4</f>
+        <f t="shared" ref="B4:B13" si="0">2^A4</f>
         <v>1024</v>
       </c>
       <c r="C4" s="4">
         <v>1024</v>
       </c>
       <c r="D4" s="4">
-        <v>508832</v>
+        <v>508926</v>
       </c>
       <c r="E4" s="4">
-        <v>508832</v>
+        <v>508926</v>
       </c>
       <c r="F4" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F4:F10" si="1">(D4-E4)/1024</f>
         <v>0</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" s="4">
         <v>15</v>
       </c>
       <c r="B5" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>32768</v>
       </c>
       <c r="C5" s="4">
         <v>32768</v>
       </c>
       <c r="D5" s="4">
-        <v>508847</v>
+        <v>508926</v>
       </c>
       <c r="E5" s="4">
-        <v>508847</v>
+        <v>508923</v>
       </c>
       <c r="F5" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.9296875E-3</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6" s="4">
         <v>20</v>
       </c>
       <c r="B6" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1048576</v>
       </c>
       <c r="C6" s="4">
         <v>1048576</v>
       </c>
       <c r="D6" s="4">
-        <v>508847</v>
+        <v>508926</v>
       </c>
       <c r="E6" s="4">
-        <v>508704</v>
+        <v>508830</v>
       </c>
       <c r="F6" s="13">
-        <f t="shared" si="0"/>
-        <v>0.1396484375</v>
+        <f t="shared" si="1"/>
+        <v>9.375E-2</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A7" s="4">
         <v>25</v>
       </c>
       <c r="B7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>33554432</v>
       </c>
       <c r="C7" s="4">
         <v>33554432</v>
       </c>
       <c r="D7" s="4">
-        <v>508847</v>
+        <v>508926</v>
       </c>
       <c r="E7" s="4">
-        <v>504576</v>
+        <v>506334</v>
       </c>
       <c r="F7" s="13">
-        <f t="shared" si="0"/>
-        <v>4.1708984375</v>
+        <f t="shared" si="1"/>
+        <v>2.53125</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A8" s="4">
         <v>30</v>
       </c>
       <c r="B8" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1073741824</v>
       </c>
       <c r="C8" s="4">
         <v>1073741824</v>
       </c>
       <c r="D8" s="4">
-        <v>508847</v>
+        <v>508926</v>
       </c>
       <c r="E8" s="4">
-        <v>389919</v>
+        <v>435155</v>
       </c>
       <c r="F8" s="13">
-        <f t="shared" si="0"/>
-        <v>116.140625</v>
+        <f t="shared" si="1"/>
+        <v>72.0419921875</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A9" s="10">
         <v>31</v>
       </c>
       <c r="B9" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2147483648</v>
       </c>
       <c r="C9" s="11">
         <v>2147483648</v>
       </c>
       <c r="D9" s="11">
-        <v>508847</v>
+        <v>508926</v>
       </c>
       <c r="E9" s="11">
-        <v>287439</v>
+        <v>369589</v>
       </c>
       <c r="F9" s="14">
-        <f t="shared" si="0"/>
-        <v>216.21875</v>
+        <f t="shared" si="1"/>
+        <v>136.0712890625</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A10" s="4">
         <v>32</v>
       </c>
       <c r="B10" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4294967296</v>
       </c>
       <c r="C10" s="4">
         <v>4294967296</v>
       </c>
       <c r="D10" s="4">
-        <v>508863</v>
+        <v>508926</v>
       </c>
       <c r="E10" s="4">
-        <v>91791</v>
+        <v>238498</v>
       </c>
       <c r="F10" s="13">
-        <f t="shared" si="0"/>
-        <v>407.296875</v>
+        <f t="shared" si="1"/>
+        <v>264.08984375</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A11" s="5">
         <v>33</v>
       </c>
       <c r="B11" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8589934592</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="5">
-        <v>508847</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
       <c r="F11" s="9" t="s">
         <v>1</v>
       </c>
@@ -1491,23 +1459,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12" s="5">
         <v>63</v>
       </c>
       <c r="B12" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9.2233720368547758E+18</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="5">
-        <v>508847</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
       <c r="F12" s="9" t="s">
         <v>1</v>
       </c>
@@ -1515,29 +1477,23 @@
         <v>1</v>
       </c>
       <c r="H12" s="30" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="I12" s="30"/>
       <c r="J12" s="30"/>
       <c r="K12" s="30"/>
     </row>
-    <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A13" s="5">
         <v>100</v>
       </c>
       <c r="B13" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.2676506002282294E+30</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="5">
-        <v>508847</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
       <c r="F13" s="9" t="s">
         <v>1</v>
       </c>
@@ -1545,7 +1501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1554,7 +1510,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1563,95 +1519,94 @@
       <c r="F15" s="3"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A16" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="22"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="23"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="25"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="23"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="25"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="23"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="25"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="23"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="25"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="23"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="25"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="23"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="25"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="23"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="25"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="26"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="28"/>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A16" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="23"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A17" s="24"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="26"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A18" s="24"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="26"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A19" s="24"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="26"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A20" s="24"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="26"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A21" s="24"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="26"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A22" s="24"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="26"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A23" s="24"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="26"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A24" s="27"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="A16:G24"/>
-    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:E12 G7:G12 H12">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
@@ -1659,6 +1614,5 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>